<commit_message>
Changed Logo, just grafik works
</commit_message>
<xml_diff>
--- a/Coin/Bestellung.xlsx
+++ b/Coin/Bestellung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HERMESS_SPSoftware\HardwareLayout\Coin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6569E1-C018-42F3-BC87-48818DD68A16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F89040-4834-45CA-A06D-4C7D5CD0DB5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{F6F68C45-8DFC-4184-AF6D-A5F25C45B0C9}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:H15"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Bestellung.xlsx, HERMESS - Spaß coin fehlt noch.
</commit_message>
<xml_diff>
--- a/Coin/Bestellung.xlsx
+++ b/Coin/Bestellung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HERMESS_SPSoftware\HardwareLayout\Coin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F89040-4834-45CA-A06D-4C7D5CD0DB5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C478A9B6-5088-469D-AEAB-E41F2A52CE38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{F6F68C45-8DFC-4184-AF6D-A5F25C45B0C9}"/>
+    <workbookView xWindow="34665" yWindow="3645" windowWidth="21600" windowHeight="11385" xr2:uid="{F6F68C45-8DFC-4184-AF6D-A5F25C45B0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -432,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371C9A44-B3B4-4D30-ACB6-75B1F709CA11}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,6 +548,12 @@
         <v>4</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f>SUM(B4:B12)</f>
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding FLO/HERMESS coin, just 4 fun
</commit_message>
<xml_diff>
--- a/Coin/Bestellung.xlsx
+++ b/Coin/Bestellung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HERMESS_SPSoftware\HardwareLayout\Coin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C478A9B6-5088-469D-AEAB-E41F2A52CE38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D7BC43-C6E4-42CC-B081-89188DC14410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34665" yWindow="3645" windowWidth="21600" windowHeight="11385" xr2:uid="{F6F68C45-8DFC-4184-AF6D-A5F25C45B0C9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Bestellung Coins</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Coin TEXT:</t>
+  </si>
+  <si>
+    <t>UNIVERSITÄT  DER  BUNDESWEHR  MÜNCHEN        REXUS        FLOMESS</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,6 +510,9 @@
       <c r="B7">
         <v>5</v>
       </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">

</xml_diff>